<commit_message>
MIABIS dictionary and yaml encoding fixed
</commit_message>
<xml_diff>
--- a/data/example-data-miabis.xlsx
+++ b/data/example-data-miabis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Antonella\Desktop\bbdataeng\a-small-fhir\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{377383A7-4954-455D-8946-C06EDD3EBF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B78B86-1F2C-46E8-9AC8-3A6F197E4582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7903CEA5-AA7C-44DF-9DC5-0F9048285697}"/>
   </bookViews>
@@ -98,22 +98,25 @@
     <t>DATE_DIAGNOSIS</t>
   </si>
   <si>
-    <t>RT</t>
-  </si>
-  <si>
-    <t>TissueFFPE</t>
-  </si>
-  <si>
-    <t>TissueFrozen</t>
-  </si>
-  <si>
-    <t>-60to-85</t>
+    <t>Room temperature</t>
+  </si>
+  <si>
+    <t>-60°C to -80°C</t>
+  </si>
+  <si>
+    <t>Tissue (frozen)</t>
+  </si>
+  <si>
+    <t>Tissue (paraffin preserved)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -155,7 +158,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -178,37 +181,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -548,16 +570,16 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="J4" sqref="J2:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="9" customWidth="1"/>
     <col min="6" max="6" width="16" style="1" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="8.42578125" style="1" customWidth="1"/>
@@ -568,13 +590,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D1" s="6" t="s">
@@ -583,128 +605,128 @@
       <c r="E1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="8">
         <v>43960</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="8">
         <v>43960</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="8">
         <v>13332</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>80</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>80</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="3" t="s">
+      <c r="J2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="8">
         <v>43960</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="8">
         <v>43960</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="8">
         <v>13332</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>82</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>82</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="3" t="s">
+      <c r="J3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="11" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="8">
         <v>43960</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="8">
         <v>43960</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="8">
         <v>14097</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>80</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>80</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="9" t="s">
+      <c r="J4" s="10" t="s">
         <v>23</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>